<commit_message>
ok, best for all features is 69.42
</commit_message>
<xml_diff>
--- a/experience/test.xlsx
+++ b/experience/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Feature</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>67.12 (unigram)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (use leming, then stem)</t>
   </si>
 </sst>
 </file>
@@ -515,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +532,7 @@
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -543,7 +546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -556,8 +559,11 @@
       <c r="D2">
         <v>64.72</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>64.739999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -570,8 +576,11 @@
       <c r="D3">
         <v>65.81</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>64.400000000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -584,8 +593,14 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>67.040000000000006</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -596,7 +611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -607,7 +622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>11</v>
       </c>
@@ -617,8 +632,11 @@
       <c r="C7" s="2">
         <v>67.08</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>67.319999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -629,7 +647,7 @@
         <v>66.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>4</v>
       </c>
@@ -642,8 +660,11 @@
       <c r="D9">
         <v>66.989999999999995</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>69.42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>12</v>
       </c>
@@ -651,8 +672,8 @@
         <v>63.92</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change lab of dataset
</commit_message>
<xml_diff>
--- a/experience/test.xlsx
+++ b/experience/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Feature</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>New 552</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa lab 1 nữa</t>
   </si>
 </sst>
 </file>
@@ -466,11 +469,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G13" sqref="G13"/>
+      <selection pane="topRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +487,7 @@
     <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -506,8 +509,11 @@
       <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -529,8 +535,11 @@
       <c r="G2" s="4">
         <v>66.86</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="4">
+        <v>65.989999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -553,7 +562,7 @@
         <v>66.709999999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -575,8 +584,11 @@
       <c r="G4" s="4">
         <v>67.900000000000006</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="4">
+        <v>69.010000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -592,8 +604,11 @@
       <c r="F5" s="4">
         <v>63.613</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="4">
+        <v>69.260000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -610,13 +625,13 @@
         <v>63.87</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
@@ -624,7 +639,7 @@
       <c r="C8" s="6"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -637,7 +652,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
@@ -650,7 +665,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -668,10 +683,13 @@
         <v>66.180000000000007</v>
       </c>
       <c r="G11" s="1">
-        <v>67.95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="H11" s="4">
+        <v>69.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
@@ -684,10 +702,13 @@
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4">
-        <v>67.944999999999993</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="H12" s="4">
+        <v>69.83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -699,11 +720,11 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ok, best with 70.
</commit_message>
<xml_diff>
--- a/experience/test.xlsx
+++ b/experience/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Feature</t>
   </si>
@@ -79,6 +79,66 @@
   </si>
   <si>
     <t>70.54 (c=28)</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>66.76 (c=32)</t>
+  </si>
+  <si>
+    <t>67.24 (c=31)</t>
+  </si>
+  <si>
+    <t>69.96 (c=29)</t>
+  </si>
+  <si>
+    <t>69.68 (c=22)</t>
+  </si>
+  <si>
+    <t>70.21 (c=27)</t>
+  </si>
+  <si>
+    <t>69.14 (c=27)</t>
+  </si>
+  <si>
+    <t>relabel 2</t>
+  </si>
+  <si>
+    <t>67.81 (c=33)</t>
+  </si>
+  <si>
+    <t>67.02 (c=29)</t>
+  </si>
+  <si>
+    <t>68.64 (c=29)</t>
+  </si>
+  <si>
+    <t>69.52 (c=32)</t>
+  </si>
+  <si>
+    <t>68.65 (29)</t>
+  </si>
+  <si>
+    <t>67.57 (c=33)</t>
+  </si>
+  <si>
+    <t>68.32 (c=34)</t>
+  </si>
+  <si>
+    <t>70.88 (c=26)</t>
+  </si>
+  <si>
+    <t>70.06 (c=33)</t>
+  </si>
+  <si>
+    <t>69.76 (c=34)</t>
   </si>
 </sst>
 </file>
@@ -162,7 +222,274 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -173,6 +500,27 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:L27" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:L27"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="Feature" dataDxfId="11"/>
+    <tableColumn id="2" name="Bài báo nền" dataDxfId="10"/>
+    <tableColumn id="3" name="Dataset khoảng 350 câu" dataDxfId="9"/>
+    <tableColumn id="4" name="Dataset 594 câu" dataDxfId="8"/>
+    <tableColumn id="5" name="Dataset 700 câu" dataDxfId="7"/>
+    <tableColumn id="6" name="New 370" dataDxfId="6"/>
+    <tableColumn id="7" name="New 552" dataDxfId="5"/>
+    <tableColumn id="8" name="Chỉnh sửa lab 1 nữa" dataDxfId="4"/>
+    <tableColumn id="9" name="relabel 2" dataDxfId="3"/>
+    <tableColumn id="10" name="Column2" dataDxfId="2"/>
+    <tableColumn id="11" name="Column3" dataDxfId="1"/>
+    <tableColumn id="12" name="Column4" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -472,25 +820,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H13" sqref="H13"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="9"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="2" max="2" width="12.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="4" customWidth="1"/>
+    <col min="4" max="5" width="16.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="19" style="4" customWidth="1"/>
+    <col min="9" max="12" width="10" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -515,8 +865,20 @@
       <c r="H1" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -538,11 +900,14 @@
       <c r="G2" s="4">
         <v>66.86</v>
       </c>
-      <c r="H2" s="4">
-        <v>65.989999999999995</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -564,8 +929,14 @@
       <c r="G3" s="4">
         <v>66.709999999999994</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -587,11 +958,14 @@
       <c r="G4" s="4">
         <v>67.900000000000006</v>
       </c>
-      <c r="H4" s="4">
-        <v>69.010000000000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -607,11 +981,14 @@
       <c r="F5" s="4">
         <v>63.613</v>
       </c>
-      <c r="H5" s="4">
-        <v>69.260000000000005</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -627,14 +1004,20 @@
       <c r="F6" s="4">
         <v>63.87</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
@@ -642,7 +1025,7 @@
       <c r="C8" s="6"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -654,8 +1037,11 @@
         <v>65.930000000000007</v>
       </c>
       <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
@@ -667,8 +1053,11 @@
         <v>66.5</v>
       </c>
       <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -688,11 +1077,14 @@
       <c r="G11" s="1">
         <v>68.099999999999994</v>
       </c>
-      <c r="H11" s="4">
-        <v>69.75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
@@ -707,14 +1099,14 @@
       <c r="G12" s="4">
         <v>67.900000000000006</v>
       </c>
-      <c r="H12" s="4">
-        <v>69.83</v>
+      <c r="H12" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -725,12 +1117,15 @@
         <v>68.7</v>
       </c>
       <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -746,5 +1141,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
phien ban dang viet report
</commit_message>
<xml_diff>
--- a/experience/test.xlsx
+++ b/experience/test.xlsx
@@ -8,6 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="141">
   <si>
     <t>Feature</t>
   </si>
@@ -144,20 +147,311 @@
     <t>NEGATION METAMAP</t>
   </si>
   <si>
-    <t>NEGATION</t>
-  </si>
-  <si>
-    <t>0.702310237286 with c=31</t>
-  </si>
-  <si>
-    <t>0.702768238363 with c=32</t>
+    <t>NEGATION 2</t>
+  </si>
+  <si>
+    <t>Thay nhan NEGATION</t>
+  </si>
+  <si>
+    <t>VECTOR</t>
+  </si>
+  <si>
+    <t>Unigram (F, min_df=1)</t>
+  </si>
+  <si>
+    <t>Unigram (P, min_df=1)</t>
+  </si>
+  <si>
+    <t>Unigram (F, min_df=2)</t>
+  </si>
+  <si>
+    <t>Unigram (F, min_df=3)</t>
+  </si>
+  <si>
+    <t>Unigram (P, min_df=2)</t>
+  </si>
+  <si>
+    <t>Unigram (P, min_df=3)</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>array([ 0.44618764,  0.64252443,  0.73528455])</t>
+  </si>
+  <si>
+    <t>array([ 0.3722218 ,  0.77317258,  0.62314163])</t>
+  </si>
+  <si>
+    <t>array([ 0.39924381,  0.69998124,  0.67225149])</t>
+  </si>
+  <si>
+    <t>array([ 0.41018398,  0.67821611,  0.71418323])</t>
+  </si>
+  <si>
+    <t>array([ 0.41702847,  0.70277772,  0.68800493])</t>
+  </si>
+  <si>
+    <t>array([ 0.40178188,  0.68717053,  0.69760058])</t>
+  </si>
+  <si>
+    <t>array([ 0.38410016,  0.67792511,  0.73271213])</t>
+  </si>
+  <si>
+    <t>array([ 0.43402472,  0.69956917,  0.6822951 ])</t>
+  </si>
+  <si>
+    <t>array([ 0.39930872,  0.68584449,  0.70315163])</t>
+  </si>
+  <si>
+    <t>Bigram (P, min_df=3)</t>
+  </si>
+  <si>
+    <t>Trigram (P, min_df=3)</t>
+  </si>
+  <si>
+    <t>Unigram (P, min_df=4)</t>
+  </si>
+  <si>
+    <t>Unigram (P, min_df=5)</t>
+  </si>
+  <si>
+    <t>array([ 0.45545183,  0.64350213,  0.73604334])</t>
+  </si>
+  <si>
+    <t>array([ 0.37993576,  0.77359704,  0.62758704])</t>
+  </si>
+  <si>
+    <t>array([ 0.40501201,  0.70046795,  0.67438646])</t>
+  </si>
+  <si>
+    <t>array([ 0.37041231,  0.68461702,  0.75199235])</t>
+  </si>
+  <si>
+    <t>array([ 0.42529331,  0.70836245,  0.69346285])</t>
+  </si>
+  <si>
+    <t>array([ 0.38783826,  0.69427691,  0.71916486])</t>
+  </si>
+  <si>
+    <t>array([ 0.3578862 ,  0.67428694,  0.75198441])</t>
+  </si>
+  <si>
+    <t>array([ 0.43696016,  0.698393  ,  0.67588572])</t>
+  </si>
+  <si>
+    <t>array([ 0.38695014,  0.68386721,  0.70929472])</t>
+  </si>
+  <si>
+    <t>min_df=1</t>
+  </si>
+  <si>
+    <t>min_df=2</t>
+  </si>
+  <si>
+    <t>min_df=3</t>
+  </si>
+  <si>
+    <t>Tri + 4 gram (P, min_df=3)</t>
+  </si>
+  <si>
+    <t>Unigram (F, min_df=4)</t>
+  </si>
+  <si>
+    <t>Unigram (F, min_df=5)</t>
+  </si>
+  <si>
+    <t>array([ 0.35726392,  0.67239393,  0.74123113])</t>
+  </si>
+  <si>
+    <t>array([ 0.4766169 ,  0.68025436,  0.66016635])</t>
+  </si>
+  <si>
+    <t>array([ 0.40078578,  0.67315888,  0.69523068])</t>
+  </si>
+  <si>
+    <t>array([ 0.37494145,  0.67613977,  0.74134727])</t>
+  </si>
+  <si>
+    <t>array([ 0.46795663,  0.69036216,  0.67419235])</t>
+  </si>
+  <si>
+    <t>array([ 0.40902103,  0.68067417,  0.70330246])</t>
+  </si>
+  <si>
+    <t>min_df=4</t>
+  </si>
+  <si>
+    <t>min_df=5</t>
+  </si>
+  <si>
+    <t>unigram</t>
+  </si>
+  <si>
+    <t>bigram</t>
+  </si>
+  <si>
+    <t>(0.68719596972408248, 0.67826262626262612, 0.67772695886226686, array([ 0.45325457,  0.67765779,  0.75361831]), array([ 0.42800722,  0.75493515,  0.68269147]), array([ 0.43148715,  0.71181172,  0.71379366]))</t>
+  </si>
+  <si>
+    <t>trigram</t>
+  </si>
+  <si>
+    <t>(0.68680989292550465, 0.68000327600327604, 0.67868942965653289, array([ 0.45606058,  0.67863171,  0.75166986]), array([ 0.42247167,  0.76007238,  0.68216021]), array([ 0.42912432,  0.71541091,  0.71329787]))</t>
+  </si>
+  <si>
+    <t>4gram</t>
+  </si>
+  <si>
+    <t>5gram</t>
+  </si>
+  <si>
+    <t>(0.68760167812499418, 0.68085339885339891, 0.67961736446250087, array([ 0.45048914,  0.68045154,  0.75352121]), array([ 0.4155437 ,  0.75612242,  0.69070894]), array([ 0.42428774,  0.7140493 ,  0.71837851]))</t>
+  </si>
+  <si>
+    <t>(0.68811135247415367, 0.67981981981981987, 0.67858342312102482, array([ 0.45753883,  0.67654792,  0.75554052]), array([ 0.41546845,  0.76457642,  0.68009642]), array([ 0.42897072,  0.715068  ,  0.71318913]))</t>
+  </si>
+  <si>
+    <t>(0.6820001058004449, 0.66871635271635266, 0.67086212890165942, ,, )</t>
+  </si>
+  <si>
+    <t>array([ 0.39894982,  0.68654095,  0.7501479 ])</t>
+  </si>
+  <si>
+    <t>array([ 0.42551098,  0.72962676,  0.69436032])</t>
+  </si>
+  <si>
+    <t>array([ 0.40418018,  0.70544668,  0.71889243])</t>
+  </si>
+  <si>
+    <t>array([ 0.41997735,  0.67501664,  0.75563614])</t>
+  </si>
+  <si>
+    <t>array([ 0.40805143,  0.75402589,  0.67783721])</t>
+  </si>
+  <si>
+    <t>array([ 0.40543812,  0.71005366,  0.71229224])</t>
+  </si>
+  <si>
+    <t>Unigram</t>
+  </si>
+  <si>
+    <t>Bigram</t>
+  </si>
+  <si>
+    <t>Trigram</t>
+  </si>
+  <si>
+    <t>4-gram</t>
+  </si>
+  <si>
+    <t>5-gram</t>
+  </si>
+  <si>
+    <t>Them tag  _NEG</t>
+  </si>
+  <si>
+    <t>1&amp;2</t>
+  </si>
+  <si>
+    <t>1&amp;3</t>
+  </si>
+  <si>
+    <t>2&amp;3</t>
+  </si>
+  <si>
+    <t>1&amp;2&amp;3</t>
+  </si>
+  <si>
+    <t>Chương 1,2,3 OK</t>
+  </si>
+  <si>
+    <t>Chương 4: Phương pháp đề xuất</t>
+  </si>
+  <si>
+    <t>Mô tả bài toán</t>
+  </si>
+  <si>
+    <t>Kiến trúc tổng quan</t>
+  </si>
+  <si>
+    <t>Các đặc trưng cơ bản</t>
+  </si>
+  <si>
+    <t>Đặc trưng mở rộng SO-CAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chương 5: </t>
+  </si>
+  <si>
+    <t>(0.69355093110608057, 0.68526835926835938, 0.6844814191533517, array([ 0.47892537,  0.67922822,  0.75937408]), array([ 0.45768714,  0.75943933,  0.68559474]), array([ 0.45943032,  0.71450683,  0.71850712]))</t>
+  </si>
+  <si>
+    <t>(0.69566445976595415, 0.68665465465465469, 0.6860399246383363, array([ 0.4860612 ,  0.68004601,  0.76024681]), array([ 0.46433251,  0.7594992 ,  0.68711777]), array([ 0.46598861,  0.71528003,  0.71903712]))</t>
+  </si>
+  <si>
+    <t>(0.68930740908095012, 0.67910838110838101, 0.67881306251505535, array([ 0.4520227 ,  0.67887993,  0.75434327]), array([ 0.43241184,  0.75718517,  0.681083  ]), array([ 0.43339486,  0.71284096,  0.71315994]))</t>
+  </si>
+  <si>
+    <t>(0.68879512942855281, 0.68103630903630896, 0.68092771720345457, array([ 0.46275166,  0.68165787,  0.75113719]), array([ 0.4444862 ,  0.74563303,  0.69037721]), array([ 0.44566349,  0.71042574,  0.71715686]))</t>
+  </si>
+  <si>
+    <t>(0.69414352478562713, 0.6854900354900354, 0.68563455479547064, array([ 0.47603026,  0.68303746,  0.75883859]), array([ 0.46854051,  0.75249947,  0.68908907]), array([ 0.46475169,  0.7139773 ,  0.72028479]))</t>
+  </si>
+  <si>
+    <t>(0.68843454786112657, 0.68019492219492217, 0.67931914319774278, array([ 0.4579742 ,  0.67894164,  0.75428127]), array([ 0.42770972,  0.76060993,  0.68094023]), array([ 0.43365856,  0.7155424 ,  0.71327289]))</t>
+  </si>
+  <si>
+    <t>(0.69351466455735711, 0.68404258804258811, 0.68442222396283425, array([ 0.46207624,  0.68674149,  0.75585147]), array([ 0.4550883 ,  0.74912377,  0.69222926]), array([ 0.44944361,  0.71436694,  0.72035374]))</t>
+  </si>
+  <si>
+    <t>(0.69585115735710157, 0.68321157521157516, 0.68499318293193068, array([ 0.46308934,  0.68388241,  0.76354407]), array([ 0.49285867,  0.73538566,  0.69483251]), array([ 0.4713668 ,  0.7056949 ,  0.72450927]))</t>
+  </si>
+  <si>
+    <t>(0.70071551060573434, 0.68983619983619959, 0.69093319498260997, array([ 0.48980221,  0.68644127,  0.76510278]), array([ 0.50252702,  0.73875543,  0.7029843 ]), array([ 0.48609153,  0.70911856,  0.73018792]))</t>
+  </si>
+  <si>
+    <t>(0.69113397220546002, 0.68121375921375948, 0.68028387033916471, array([ 0.43898482,  0.67326493,  0.77040173]), array([ 0.41240977,  0.76725157,  0.68176394]), array([ 0.41773196,  0.71459839,  0.72069121]))</t>
+  </si>
+  <si>
+    <t>(0.69953968408927314, 0.68635271635271633, 0.68818624579973653, array([ 0.47455546,  0.68180627,  0.77291628]), array([ 0.52393745,  0.74261705,  0.68437578]), array([ 0.49093472,  0.70862411,  0.72338086]))</t>
+  </si>
+  <si>
+    <t>(0.69473824507437054, 0.67852306852306854, 0.68155674961305268, array([ 0.42977083,  0.67749975,  0.78125355]), array([ 0.50170501,  0.736598  ,  0.68000345]), array([ 0.45557068,  0.70369832,  0.72496027]))</t>
+  </si>
+  <si>
+    <t>(0.68999316354592399, 0.67996614796614785, 0.67830598374451578, array([ 0.4583481 ,  0.66795021,  0.7685256 ]), array([ 0.41654653,  0.77532359,  0.66999416]), array([ 0.42802475,  0.71536041,  0.71320833]))</t>
+  </si>
+  <si>
+    <t>(0.69618215315555942, 0.67955555555555569, 0.6821731152989684, array([ 0.44111862,  0.67788173,  0.77696032]), array([ 0.50201504,  0.73995844,  0.68009998]), array([ 0.45951191,  0.70501588,  0.72253122]))</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>(0.69130914561711199, 0.68223805623805611, 0.68274758511466793, array([ 0.44916171,  0.68878273,  0.75069852]), array([ 0.43875086,  0.73944362,  0.7029949 ]), array([ 0.43714223,  0.71079512,  0.72287246]))</t>
+  </si>
+  <si>
+    <t>(0.70841313698324093, 0.70049030849030847, 0.70033995487667311, array([ 0.4877358 ,  0.70034624,  0.76834711]), array([ 0.46337451,  0.76515677,  0.71106585]), array([ 0.4690288 ,  0.72905097,  0.73602816]))</t>
+  </si>
+  <si>
+    <t>(0.716412959967068, 0.70700136500136468, 0.70742754403914543, array([ 0.52200776,  0.70063298,  0.77762601]), array([ 0.51892349,  0.77018145,  0.70544719]), array([ 0.51167325,  0.73158988,  0.73806379]))</t>
+  </si>
+  <si>
+    <t>(0.71489306289788368, 0.70544253344253349, 0.70596317121777297, array([ 0.50575936,  0.70667562,  0.77118519]), array([ 0.50831397,  0.76105334,  0.71616551]), array([ 0.49794664,  0.73048968,  0.73997746]))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +488,15 @@
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -215,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -230,6 +533,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,22 +818,2761 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$M$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>F</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="ltDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$L$24:$L$28</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>min_df=1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>min_df=2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>min_df=3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>min_df=4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>min_df=5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$M$24:$M$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>65.055476005974597</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65.591827604229209</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65.7958359102266</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65.619721318882796</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64.916616117245795</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1C36-4EA7-8130-3CEAE22EAD46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$N$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$L$24:$L$28</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>min_df=1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>min_df=2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>min_df=3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>min_df=4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>min_df=5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$N$24:$N$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>65.229300139581397</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67.261564577485203</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.315332754780002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66.7141028723575</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65.788814941824199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1C36-4EA7-8130-3CEAE22EAD46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="375654480"/>
+        <c:axId val="375648248"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="375654480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="375648248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="375648248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>F-measure</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="375654480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$D$20:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>67.315332754780002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67.7726958862266</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.868942965653204</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67.961736446250001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.858342312102408</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3015-4956-B319-55F45CC86D9A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="328781832"/>
+        <c:axId val="328784128"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="328781832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="328784128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="328784128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="328781832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$C$20:$C$24</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Unigram</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bigram</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Trigram</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4-gram</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5-gram</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$D$20:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>67.315332754780002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67.7726958862266</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.868942965653204</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67.961736446250001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.858342312102408</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-826A-4C83-9FED-ADB0B46154E1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="334687072"/>
+        <c:axId val="334687400"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="334687072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334687400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="334687400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="68.2"/>
+          <c:min val="67"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>F-measure</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="334687072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142877</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>248365</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>56658</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D02ABE6-9D3F-4707-A821-2C1041FFD36B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C6A3A01-C366-4516-8379-DBDB0F908C36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>366711</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>274636</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56A9FA01-BF0E-4155-A63F-9DF2071102BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:L27" totalsRowShown="0" headerRowDxfId="13" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:L27" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:L27"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Feature" dataDxfId="12"/>
-    <tableColumn id="2" name="Bài báo nền" dataDxfId="11"/>
-    <tableColumn id="3" name="Dataset khoảng 350 câu" dataDxfId="10"/>
-    <tableColumn id="4" name="Dataset 594 câu" dataDxfId="9"/>
-    <tableColumn id="5" name="Dataset 700 câu" dataDxfId="8"/>
-    <tableColumn id="6" name="New 370" dataDxfId="7"/>
-    <tableColumn id="7" name="New 552" dataDxfId="6"/>
-    <tableColumn id="8" name="Chỉnh sửa lab 1 nữa" dataDxfId="5"/>
-    <tableColumn id="9" name="relabel 2" dataDxfId="4"/>
-    <tableColumn id="10" name="Column2" dataDxfId="3"/>
-    <tableColumn id="11" name="Column3" dataDxfId="2"/>
-    <tableColumn id="12" name="Column4" dataDxfId="1"/>
+    <tableColumn id="1" name="Feature" dataDxfId="11"/>
+    <tableColumn id="2" name="Bài báo nền" dataDxfId="10"/>
+    <tableColumn id="3" name="Dataset khoảng 350 câu" dataDxfId="9"/>
+    <tableColumn id="4" name="Dataset 594 câu" dataDxfId="8"/>
+    <tableColumn id="5" name="Dataset 700 câu" dataDxfId="7"/>
+    <tableColumn id="6" name="New 370" dataDxfId="6"/>
+    <tableColumn id="7" name="New 552" dataDxfId="5"/>
+    <tableColumn id="8" name="Chỉnh sửa lab 1 nữa" dataDxfId="4"/>
+    <tableColumn id="9" name="relabel 2" dataDxfId="3"/>
+    <tableColumn id="10" name="Column2" dataDxfId="2"/>
+    <tableColumn id="11" name="Column3" dataDxfId="1"/>
+    <tableColumn id="12" name="Column4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -836,7 +3879,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J20" sqref="J20"/>
+      <selection pane="topRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +3891,8 @@
     <col min="6" max="6" width="10.28515625" style="9" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" style="4" customWidth="1"/>
     <col min="8" max="8" width="19" style="4" customWidth="1"/>
-    <col min="9" max="12" width="10" style="4" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="4" customWidth="1"/>
+    <col min="10" max="12" width="10" style="4" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -999,9 +4043,6 @@
       <c r="I5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="4">
-        <v>70276</v>
-      </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1071,6 +4112,9 @@
       <c r="I10" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="J10" s="4" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -1098,6 +4142,9 @@
       <c r="I11" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="J11" s="4" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -1120,6 +4167,9 @@
       <c r="I12" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="J12" s="4" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1135,6 +4185,9 @@
       <c r="I13" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="J13" s="4" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F14" s="4"/>
@@ -1146,50 +4199,32 @@
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F18" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="6:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1197,4 +4232,746 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="10"/>
+      <c r="E9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N28"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2">
+        <v>0.66210065158600095</v>
+      </c>
+      <c r="G2">
+        <v>0.65463663663663596</v>
+      </c>
+      <c r="H2">
+        <v>0.650554760059746</v>
+      </c>
+      <c r="K2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3">
+        <v>0.66555748408173199</v>
+      </c>
+      <c r="G3">
+        <v>0.65623587223587199</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0.65229300139581403</v>
+      </c>
+      <c r="K3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4">
+        <v>0.66500228540716699</v>
+      </c>
+      <c r="G4">
+        <v>0.65550969150969096</v>
+      </c>
+      <c r="H4">
+        <v>0.65591827604229203</v>
+      </c>
+      <c r="K4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5">
+        <v>0.68218269678274202</v>
+      </c>
+      <c r="G5">
+        <v>0.67310728910728901</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0.672615645774852</v>
+      </c>
+      <c r="K5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6">
+        <v>0.66980065739327799</v>
+      </c>
+      <c r="G6">
+        <v>0.65476876876876799</v>
+      </c>
+      <c r="H6">
+        <v>0.65795835910226597</v>
+      </c>
+      <c r="K6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7">
+        <v>0.68121018464223904</v>
+      </c>
+      <c r="G7">
+        <v>0.67228719628719602</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0.6731533275478</v>
+      </c>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8">
+        <v>0.67015187860013903</v>
+      </c>
+      <c r="G8">
+        <v>0.651272727272727</v>
+      </c>
+      <c r="H8">
+        <v>0.65619721318882795</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9">
+        <v>0.67833254105859198</v>
+      </c>
+      <c r="G9">
+        <v>0.66335408135408103</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0.66714102872357495</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10">
+        <v>0.66751105952845002</v>
+      </c>
+      <c r="G10">
+        <v>0.64208408408408402</v>
+      </c>
+      <c r="H10">
+        <v>0.64916616117245796</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11">
+        <v>0.67184453764886398</v>
+      </c>
+      <c r="G11">
+        <v>0.65266448266448196</v>
+      </c>
+      <c r="H11" s="10">
+        <v>0.65788814941824203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13">
+        <v>0.67772695886226597</v>
+      </c>
+      <c r="I13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14">
+        <v>0.67868942965653201</v>
+      </c>
+      <c r="I14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15">
+        <v>0.67961736446249998</v>
+      </c>
+      <c r="I15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="H16">
+        <v>0.67858342312102404</v>
+      </c>
+      <c r="I16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="10">
+        <f>100*E20</f>
+        <v>67.315332754780002</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0.6731533275478</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="10">
+        <f t="shared" ref="D21:D24" si="0">100*E21</f>
+        <v>67.7726958862266</v>
+      </c>
+      <c r="E21">
+        <v>0.67772695886226597</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="10">
+        <f t="shared" si="0"/>
+        <v>67.868942965653204</v>
+      </c>
+      <c r="E22">
+        <v>0.67868942965653201</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23" s="10">
+        <f t="shared" si="0"/>
+        <v>67.961736446250001</v>
+      </c>
+      <c r="E23">
+        <v>0.67961736446249998</v>
+      </c>
+      <c r="M23" t="s">
+        <v>52</v>
+      </c>
+      <c r="N23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="10">
+        <f t="shared" si="0"/>
+        <v>67.858342312102408</v>
+      </c>
+      <c r="E24">
+        <v>0.67858342312102404</v>
+      </c>
+      <c r="J24">
+        <v>0.650554760059746</v>
+      </c>
+      <c r="K24" s="10">
+        <v>0.65229300139581403</v>
+      </c>
+      <c r="L24" t="s">
+        <v>75</v>
+      </c>
+      <c r="M24">
+        <f>100*J24</f>
+        <v>65.055476005974597</v>
+      </c>
+      <c r="N24">
+        <f>100*K24</f>
+        <v>65.229300139581397</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>0.65591827604229203</v>
+      </c>
+      <c r="K25" s="10">
+        <v>0.672615645774852</v>
+      </c>
+      <c r="L25" t="s">
+        <v>76</v>
+      </c>
+      <c r="M25">
+        <f t="shared" ref="M25:M28" si="1">100*J25</f>
+        <v>65.591827604229209</v>
+      </c>
+      <c r="N25">
+        <f t="shared" ref="N25:N28" si="2">100*K25</f>
+        <v>67.261564577485203</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>0.65795835910226597</v>
+      </c>
+      <c r="K26" s="10">
+        <v>0.6731533275478</v>
+      </c>
+      <c r="L26" t="s">
+        <v>77</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="1"/>
+        <v>65.7958359102266</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="2"/>
+        <v>67.315332754780002</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>0.65619721318882795</v>
+      </c>
+      <c r="K27" s="10">
+        <v>0.66714102872357495</v>
+      </c>
+      <c r="L27" t="s">
+        <v>87</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="1"/>
+        <v>65.619721318882796</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="2"/>
+        <v>66.7141028723575</v>
+      </c>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <v>0.64916616117245796</v>
+      </c>
+      <c r="K28" s="10">
+        <v>0.65788814941824203</v>
+      </c>
+      <c r="L28" t="s">
+        <v>88</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="1"/>
+        <v>64.916616117245795</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="2"/>
+        <v>65.788814941824199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>